<commit_message>
Changed pantry to display ingredients in responsive grid
Changed the layout of pantry to display the ingredients in a grid
Placed the add new ingredient form at the top outside of the scrollable
ingredient grid.
</commit_message>
<xml_diff>
--- a/sprints/Sprint1/Sprint 1 Backlog Burndown Chart.xlsx
+++ b/sprints/Sprint1/Sprint 1 Backlog Burndown Chart.xlsx
@@ -365,11 +365,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="247044657"/>
-        <c:axId val="1557453570"/>
+        <c:axId val="543568590"/>
+        <c:axId val="798122615"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="247044657"/>
+        <c:axId val="543568590"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -421,10 +421,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1557453570"/>
+        <c:crossAx val="798122615"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1557453570"/>
+        <c:axId val="798122615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,7 +488,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247044657"/>
+        <c:crossAx val="543568590"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -914,9 +914,7 @@
       <c r="E10" s="10">
         <v>2.0</v>
       </c>
-      <c r="F10" s="10">
-        <v>0.0</v>
-      </c>
+      <c r="F10" s="12"/>
     </row>
     <row r="11">
       <c r="A11" s="8"/>
@@ -932,9 +930,7 @@
       <c r="E11" s="10">
         <v>2.0</v>
       </c>
-      <c r="F11" s="10">
-        <v>2.0</v>
-      </c>
+      <c r="F11" s="12"/>
     </row>
     <row r="12">
       <c r="A12" s="8"/>
@@ -996,9 +992,7 @@
       <c r="E15" s="10">
         <v>0.0</v>
       </c>
-      <c r="F15" s="10">
-        <v>0.0</v>
-      </c>
+      <c r="F15" s="12"/>
     </row>
     <row r="16">
       <c r="A16" s="8"/>
@@ -1014,9 +1008,7 @@
       <c r="E16" s="10">
         <v>0.0</v>
       </c>
-      <c r="F16" s="10">
-        <v>0.0</v>
-      </c>
+      <c r="F16" s="12"/>
     </row>
     <row r="17">
       <c r="A17" s="8"/>
@@ -1032,9 +1024,7 @@
       <c r="E17" s="10">
         <v>1.0</v>
       </c>
-      <c r="F17" s="10">
-        <v>0.0</v>
-      </c>
+      <c r="F17" s="12"/>
     </row>
     <row r="18">
       <c r="A18" s="8"/>
@@ -1173,12 +1163,8 @@
       <c r="D25" s="9">
         <v>2.0</v>
       </c>
-      <c r="E25" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="F25" s="10">
-        <v>0.0</v>
-      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="8"/>
@@ -1271,9 +1257,7 @@
       <c r="D32" s="8">
         <v>1.0</v>
       </c>
-      <c r="E32" s="10">
-        <v>1.0</v>
-      </c>
+      <c r="E32" s="12"/>
       <c r="F32" s="12"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -1290,9 +1274,7 @@
       <c r="E33" s="10">
         <v>0.0</v>
       </c>
-      <c r="F33" s="10">
-        <v>0.0</v>
-      </c>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="8"/>
@@ -1308,9 +1290,7 @@
       <c r="E34" s="10">
         <v>0.0</v>
       </c>
-      <c r="F34" s="10">
-        <v>0.0</v>
-      </c>
+      <c r="F34" s="12"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="8"/>
@@ -1344,9 +1324,7 @@
       <c r="E36" s="10">
         <v>0.0</v>
       </c>
-      <c r="F36" s="10">
-        <v>0.0</v>
-      </c>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="8"/>
@@ -1377,11 +1355,9 @@
         <v>2.0</v>
       </c>
       <c r="E38" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="F38" s="10">
-        <v>0.0</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="F38" s="12"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="B39" s="15" t="s">
@@ -1394,11 +1370,11 @@
       </c>
       <c r="E39" s="16">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F39" s="16">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>

</xml_diff>